<commit_message>
New page O model
</commit_message>
<xml_diff>
--- a/PageObjectModel_Javab/src/test/resources/excel/testdata.xlsx
+++ b/PageObjectModel_Javab/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkumar\eclipse-workspace\PageObjectModel_Javab\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C5E36C-92EC-4C32-BB2B-FF2BB4BFBC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{BF5B4E46-44B5-4D3F-8269-43C75D271B63}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="verifyAvailablePets" sheetId="7" r:id="rId1"/>
@@ -20,7 +14,7 @@
     <sheet name="Verifylogin" sheetId="3" r:id="rId5"/>
     <sheet name="verifyAllPets" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="9">
   <si>
     <t>browser</t>
   </si>
@@ -50,12 +44,6 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>edge</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -74,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,7 +154,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -218,7 +206,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -412,23 +400,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C004D3-FCE3-4D63-A849-EC420EFBE89E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,7 +429,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -453,16 +441,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC575E-2D79-4337-A157-72DD7221D84E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -487,16 +475,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E57EBF8-1CA0-48E8-9CD5-659F1252CD28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -521,14 +509,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1769F7FB-81AA-49E7-A3EB-EC3A1E2D75C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
   </cols>
@@ -543,7 +531,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -555,14 +543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1815237A-57FA-4EF4-B49E-788B6EB767BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -572,10 +560,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -586,24 +574,24 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -614,24 +602,24 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -640,14 +628,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54084210-C66C-451D-B938-DD5802E2269F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>